<commit_message>
adding CapStatement for DEQM
</commit_message>
<xml_diff>
--- a/CapStatement/Argonaut_Capability_Statement_CLIENT_Clinical_Notes.xlsx
+++ b/CapStatement/Argonaut_Capability_Statement_CLIENT_Clinical_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/CapStatement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BF467E-211B-4143-A62A-97F9AD6AF7F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029B9285-23CE-3747-B57D-612C05B3A687}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="5" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
   <si>
     <t>Value</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>patient,category,code</t>
+  </si>
+  <si>
+    <t>- The search parameters `created`, `class`, and `type`  MAY NOT be available as a *single* search parameter but SHALL be available in the combinations listed below.</t>
+  </si>
+  <si>
+    <t>- The search parameters `date`, `category`, and  `code`  MAY NOT be available as a *single* search parameter but SHALL be available in the combinations listed below.</t>
   </si>
 </sst>
 </file>
@@ -846,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB4CFA-AAEF-4FC6-A49B-107CEE80A317}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -859,6 +865,7 @@
     <col min="5" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -890,26 +897,30 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="I3" t="s">
         <v>83</v>
       </c>
@@ -1083,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>